<commit_message>
Refactor export service to support chunk query with only one iteration
</commit_message>
<xml_diff>
--- a/sample/Hsu.Db.Export.Spreadsheet.Worker/ExportTemplate.xlsx
+++ b/sample/Hsu.Db.Export.Spreadsheet.Worker/ExportTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\hsu\Hsu.Db.Export.Spreadsheet\sample\Hsu.Db.Export.Spreadsheet.Worker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADBA10F-60FA-4963-AC78-F968DE30BADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53995EC8-7073-49EA-BBE6-60CFB9041A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="4830" windowWidth="21600" windowHeight="11295" xr2:uid="{F13CCE45-E46F-41E8-AD69-EBD278FD6C2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F13CCE45-E46F-41E8-AD69-EBD278FD6C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>{{_.EmployeeNo}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>EmployeeNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,15 +44,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{_.Salary}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FromDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{_.FromDate}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -64,15 +52,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{_.ToDate}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Create At</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{_.create_at}}</t>
+    <t>create_at</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,12 +81,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -134,11 +124,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,7 +451,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -471,20 +464,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -492,16 +485,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>